<commit_message>
correct ID column typo
</commit_message>
<xml_diff>
--- a/dataset05-cropping-table-babb02.1,babb03-no_tail-filled.xlsx
+++ b/dataset05-cropping-table-babb02.1,babb03-no_tail-filled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\imageProcessTif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8115B87-2356-426E-8C27-231F3E75A914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87F4C74-7B74-47CD-8672-EB454B752F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="45">
   <si>
     <t>dataset</t>
   </si>
@@ -134,6 +134,27 @@
   </si>
   <si>
     <t>babb03</t>
+  </si>
+  <si>
+    <t>id01</t>
+  </si>
+  <si>
+    <t>id02</t>
+  </si>
+  <si>
+    <t>id03</t>
+  </si>
+  <si>
+    <t>id04</t>
+  </si>
+  <si>
+    <t>id05</t>
+  </si>
+  <si>
+    <t>id06</t>
+  </si>
+  <si>
+    <t>id07</t>
   </si>
 </sst>
 </file>
@@ -498,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,8 +639,8 @@
       <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="G2">
-        <v>1</v>
+      <c r="G2" t="s">
+        <v>38</v>
       </c>
       <c r="H2">
         <v>260</v>
@@ -713,8 +734,8 @@
       <c r="F3" t="s">
         <v>36</v>
       </c>
-      <c r="G3">
-        <v>2</v>
+      <c r="G3" t="s">
+        <v>39</v>
       </c>
       <c r="H3">
         <v>487</v>
@@ -808,8 +829,8 @@
       <c r="F4" t="s">
         <v>36</v>
       </c>
-      <c r="G4">
-        <v>3</v>
+      <c r="G4" t="s">
+        <v>40</v>
       </c>
       <c r="H4">
         <v>256</v>
@@ -903,8 +924,8 @@
       <c r="F5" t="s">
         <v>36</v>
       </c>
-      <c r="G5">
-        <v>4</v>
+      <c r="G5" t="s">
+        <v>41</v>
       </c>
       <c r="H5">
         <v>265</v>
@@ -998,8 +1019,8 @@
       <c r="F6" t="s">
         <v>36</v>
       </c>
-      <c r="G6">
-        <v>5</v>
+      <c r="G6" t="s">
+        <v>42</v>
       </c>
       <c r="H6">
         <v>313</v>
@@ -1093,8 +1114,8 @@
       <c r="F7" t="s">
         <v>36</v>
       </c>
-      <c r="G7">
-        <v>6</v>
+      <c r="G7" t="s">
+        <v>43</v>
       </c>
       <c r="H7">
         <v>213</v>
@@ -1188,8 +1209,8 @@
       <c r="F8" t="s">
         <v>36</v>
       </c>
-      <c r="G8">
-        <v>1</v>
+      <c r="G8" t="s">
+        <v>38</v>
       </c>
       <c r="H8">
         <v>426</v>
@@ -1283,8 +1304,8 @@
       <c r="F9" t="s">
         <v>36</v>
       </c>
-      <c r="G9">
-        <v>2</v>
+      <c r="G9" t="s">
+        <v>39</v>
       </c>
       <c r="H9">
         <v>503</v>
@@ -1378,8 +1399,8 @@
       <c r="F10" t="s">
         <v>36</v>
       </c>
-      <c r="G10">
-        <v>3</v>
+      <c r="G10" t="s">
+        <v>40</v>
       </c>
       <c r="H10">
         <v>378</v>
@@ -1473,8 +1494,8 @@
       <c r="F11" t="s">
         <v>36</v>
       </c>
-      <c r="G11">
-        <v>4</v>
+      <c r="G11" t="s">
+        <v>41</v>
       </c>
       <c r="H11">
         <v>423</v>
@@ -1568,8 +1589,8 @@
       <c r="F12" t="s">
         <v>36</v>
       </c>
-      <c r="G12">
-        <v>5</v>
+      <c r="G12" t="s">
+        <v>42</v>
       </c>
       <c r="H12">
         <v>384</v>
@@ -1663,8 +1684,8 @@
       <c r="F13" t="s">
         <v>36</v>
       </c>
-      <c r="G13">
-        <v>6</v>
+      <c r="G13" t="s">
+        <v>43</v>
       </c>
       <c r="H13">
         <v>495</v>
@@ -1758,8 +1779,8 @@
       <c r="F14" t="s">
         <v>36</v>
       </c>
-      <c r="G14">
-        <v>7</v>
+      <c r="G14" t="s">
+        <v>44</v>
       </c>
       <c r="H14">
         <v>339</v>

</xml_diff>

<commit_message>
put some static ijm input array text into archive dataset05
</commit_message>
<xml_diff>
--- a/dataset05-cropping-table-babb02.1,babb03-no_tail-filled.xlsx
+++ b/dataset05-cropping-table-babb02.1,babb03-no_tail-filled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\imageProcessTif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87F4C74-7B74-47CD-8672-EB454B752F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0F40C7-C599-4DB6-ADCE-654511B25A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,5 +1857,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>